<commit_message>
Imported arguments in workflows
</commit_message>
<xml_diff>
--- a/DataFiles/POS-TestData.xlsx
+++ b/DataFiles/POS-TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Csharmila\Documents\UiPath\POSweb\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmariam\Documents\UiPath\POSweb\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
   <si>
     <t>SalesPerson</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>TC2-Return a sales slip</t>
+  </si>
+  <si>
+    <t>TC2-Return a sales slip - Invalid Scenario</t>
   </si>
 </sst>
 </file>
@@ -455,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,6 +522,20 @@
       </c>
       <c r="E3" s="1">
         <v>20018160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5649</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1">
+        <v>740</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated negative scenario and scenario names - Sharmila
</commit_message>
<xml_diff>
--- a/DataFiles/POS-TestData.xlsx
+++ b/DataFiles/POS-TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmariam\Documents\UiPath\POSweb\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Csharmila\Documents\UiPath\POSweb\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>SalesPerson</t>
   </si>
@@ -105,10 +105,13 @@
     <t>TC1-Place an order with cash tender</t>
   </si>
   <si>
-    <t>TC2-Return a sales slip</t>
-  </si>
-  <si>
-    <t>TC2-Return a sales slip - Invalid Scenario</t>
+    <t>TC2-Get Slip from CUI</t>
+  </si>
+  <si>
+    <t>TC3-Return a sales slip</t>
+  </si>
+  <si>
+    <t>TC4-Return a sales slip - Invalid Scenario</t>
   </si>
 </sst>
 </file>
@@ -458,15 +461,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" customWidth="1"/>
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
@@ -511,18 +514,10 @@
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="1">
-        <v>5649</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1">
-        <v>740</v>
-      </c>
-      <c r="E3" s="1">
-        <v>20018160</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -537,6 +532,24 @@
       <c r="D4" s="1">
         <v>740</v>
       </c>
+      <c r="E4" s="1">
+        <v>20018160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5649</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1">
+        <v>740</v>
+      </c>
+      <c r="E5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed select all items for return not clicking - Sharmila
</commit_message>
<xml_diff>
--- a/DataFiles/POS-TestData.xlsx
+++ b/DataFiles/POS-TestData.xlsx
@@ -111,7 +111,7 @@
     <t>TC3-Return a sales slip</t>
   </si>
   <si>
-    <t>TC4-Return a sales slip - Invalid Scenario</t>
+    <t>TC4-Return a sales slip - Negative Scenario</t>
   </si>
 </sst>
 </file>
@@ -464,12 +464,12 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" customWidth="1"/>
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>

</xml_diff>